<commit_message>
added for extra feature selection
</commit_message>
<xml_diff>
--- a/Results_Worksheet.xlsx
+++ b/Results_Worksheet.xlsx
@@ -1,18 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26915"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/viveknair/GIT/Reimplement/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/viveknair/PycharmProjects/Reimplement/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16600" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Random VS WHAT" sheetId="1" r:id="rId1"/>
+    <sheet name="min_max" sheetId="2" r:id="rId2"/>
+    <sheet name="z-score" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="29">
   <si>
     <t>./Data/Apache_AllMeasurements.csv</t>
   </si>
@@ -120,7 +123,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -143,6 +146,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -161,24 +191,77 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -484,8 +567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -496,40 +579,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="4"/>
+      <c r="D1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2" t="s">
+      <c r="E1" s="4"/>
+      <c r="F1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="2"/>
+      <c r="G1" s="4"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="1"/>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="3"/>
+      <c r="B2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="1" t="s">
         <v>25</v>
       </c>
     </row>
@@ -584,7 +667,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B5">
@@ -609,7 +692,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B6">
@@ -759,7 +842,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B12">
@@ -1059,7 +1142,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B24">
@@ -1084,7 +1167,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B25">
@@ -1116,10 +1199,1845 @@
     <mergeCell ref="F1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="F3:G25">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="35.1640625" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="7"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="6"/>
+      <c r="B2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="9">
+        <v>12.193</v>
+      </c>
+      <c r="C3" s="9">
+        <v>2.9849999999999999</v>
+      </c>
+      <c r="D3" s="9">
+        <v>13.003</v>
+      </c>
+      <c r="E3" s="9">
+        <v>4.2859999999999996</v>
+      </c>
+      <c r="F3" s="9">
+        <f>D3-B3</f>
+        <v>0.8100000000000005</v>
+      </c>
+      <c r="G3" s="9">
+        <f>E3-C3</f>
+        <v>1.3009999999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="9">
+        <v>5.3650000000000002</v>
+      </c>
+      <c r="C4" s="9">
+        <v>2.8769999999999998</v>
+      </c>
+      <c r="D4" s="9">
+        <v>6.7060000000000004</v>
+      </c>
+      <c r="E4" s="9">
+        <v>2.625</v>
+      </c>
+      <c r="F4" s="9">
+        <f t="shared" ref="F4:F25" si="0">D4-B4</f>
+        <v>1.3410000000000002</v>
+      </c>
+      <c r="G4" s="9">
+        <f t="shared" ref="G4:G25" si="1">E4-C4</f>
+        <v>-0.25199999999999978</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="9">
+        <v>15.928000000000001</v>
+      </c>
+      <c r="C5" s="9">
+        <v>2.4990000000000001</v>
+      </c>
+      <c r="D5" s="9">
+        <v>14.859</v>
+      </c>
+      <c r="E5" s="9">
+        <v>1.9610000000000001</v>
+      </c>
+      <c r="F5" s="9">
+        <f t="shared" si="0"/>
+        <v>-1.0690000000000008</v>
+      </c>
+      <c r="G5" s="9">
+        <f t="shared" si="1"/>
+        <v>-0.53800000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="9">
+        <v>15.958</v>
+      </c>
+      <c r="C6" s="9">
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="D6" s="9">
+        <v>16.503</v>
+      </c>
+      <c r="E6" s="9">
+        <v>1.7609999999999999</v>
+      </c>
+      <c r="F6" s="9">
+        <f t="shared" si="0"/>
+        <v>0.54499999999999993</v>
+      </c>
+      <c r="G6" s="9">
+        <f t="shared" si="1"/>
+        <v>0.87899999999999989</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="9">
+        <v>22.062999999999999</v>
+      </c>
+      <c r="C7" s="9">
+        <v>2.085</v>
+      </c>
+      <c r="D7" s="9">
+        <v>24.094999999999999</v>
+      </c>
+      <c r="E7" s="9">
+        <v>2.6840000000000002</v>
+      </c>
+      <c r="F7" s="9">
+        <f t="shared" si="0"/>
+        <v>2.032</v>
+      </c>
+      <c r="G7" s="9">
+        <f t="shared" si="1"/>
+        <v>0.5990000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="9">
+        <v>55.116999999999997</v>
+      </c>
+      <c r="C8" s="9">
+        <v>20.523</v>
+      </c>
+      <c r="D8" s="9">
+        <v>127.29300000000001</v>
+      </c>
+      <c r="E8" s="9">
+        <v>140.01900000000001</v>
+      </c>
+      <c r="F8" s="9">
+        <f t="shared" si="0"/>
+        <v>72.176000000000016</v>
+      </c>
+      <c r="G8" s="9">
+        <f t="shared" si="1"/>
+        <v>119.49600000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="9">
+        <v>183.518</v>
+      </c>
+      <c r="C9" s="9">
+        <v>120.20699999999999</v>
+      </c>
+      <c r="D9" s="9">
+        <v>224.56800000000001</v>
+      </c>
+      <c r="E9" s="9">
+        <v>248.68799999999999</v>
+      </c>
+      <c r="F9" s="9">
+        <f t="shared" si="0"/>
+        <v>41.050000000000011</v>
+      </c>
+      <c r="G9" s="9">
+        <f t="shared" si="1"/>
+        <v>128.48099999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="9">
+        <v>366.78399999999999</v>
+      </c>
+      <c r="C10" s="9">
+        <v>426.25099999999998</v>
+      </c>
+      <c r="D10" s="9">
+        <v>1519.614</v>
+      </c>
+      <c r="E10" s="9">
+        <v>2006.152</v>
+      </c>
+      <c r="F10" s="9">
+        <f t="shared" si="0"/>
+        <v>1152.83</v>
+      </c>
+      <c r="G10" s="9">
+        <f t="shared" si="1"/>
+        <v>1579.9010000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="9">
+        <v>101.148</v>
+      </c>
+      <c r="C11" s="9">
+        <v>59.811</v>
+      </c>
+      <c r="D11" s="9">
+        <v>96.337999999999994</v>
+      </c>
+      <c r="E11" s="9">
+        <v>45.415999999999997</v>
+      </c>
+      <c r="F11" s="9">
+        <f t="shared" si="0"/>
+        <v>-4.8100000000000023</v>
+      </c>
+      <c r="G11" s="9">
+        <f t="shared" si="1"/>
+        <v>-14.395000000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="9">
+        <v>971.94399999999996</v>
+      </c>
+      <c r="C12" s="9">
+        <v>915.80399999999997</v>
+      </c>
+      <c r="D12" s="9">
+        <v>533.01599999999996</v>
+      </c>
+      <c r="E12" s="9">
+        <v>399.57900000000001</v>
+      </c>
+      <c r="F12" s="9">
+        <f t="shared" si="0"/>
+        <v>-438.928</v>
+      </c>
+      <c r="G12" s="9">
+        <f t="shared" si="1"/>
+        <v>-516.22499999999991</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="9">
+        <v>21.925000000000001</v>
+      </c>
+      <c r="C13" s="9">
+        <v>1.2230000000000001</v>
+      </c>
+      <c r="D13" s="9">
+        <v>12.611000000000001</v>
+      </c>
+      <c r="E13" s="9">
+        <v>2.1120000000000001</v>
+      </c>
+      <c r="F13" s="9">
+        <f t="shared" si="0"/>
+        <v>-9.3140000000000001</v>
+      </c>
+      <c r="G13" s="9">
+        <f t="shared" si="1"/>
+        <v>0.88900000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="9">
+        <v>5.61</v>
+      </c>
+      <c r="C14" s="9">
+        <v>0.27900000000000003</v>
+      </c>
+      <c r="D14" s="9">
+        <v>5.5810000000000004</v>
+      </c>
+      <c r="E14" s="9">
+        <v>0.64</v>
+      </c>
+      <c r="F14" s="9">
+        <f t="shared" si="0"/>
+        <v>-2.8999999999999915E-2</v>
+      </c>
+      <c r="G14" s="9">
+        <f t="shared" si="1"/>
+        <v>0.36099999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="9">
+        <v>44.442</v>
+      </c>
+      <c r="C15" s="9">
+        <v>22.497</v>
+      </c>
+      <c r="D15" s="9">
+        <v>45.036999999999999</v>
+      </c>
+      <c r="E15" s="9">
+        <v>22.574999999999999</v>
+      </c>
+      <c r="F15" s="9">
+        <f t="shared" si="0"/>
+        <v>0.59499999999999886</v>
+      </c>
+      <c r="G15" s="9">
+        <f t="shared" si="1"/>
+        <v>7.7999999999999403E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="9">
+        <v>483.68</v>
+      </c>
+      <c r="C16" s="9">
+        <v>467.68099999999998</v>
+      </c>
+      <c r="D16" s="9">
+        <v>407.05700000000002</v>
+      </c>
+      <c r="E16" s="9">
+        <v>360.76600000000002</v>
+      </c>
+      <c r="F16" s="9">
+        <f t="shared" si="0"/>
+        <v>-76.62299999999999</v>
+      </c>
+      <c r="G16" s="9">
+        <f t="shared" si="1"/>
+        <v>-106.91499999999996</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="9">
+        <v>32.792999999999999</v>
+      </c>
+      <c r="C17" s="9">
+        <v>8.2829999999999995</v>
+      </c>
+      <c r="D17" s="9">
+        <v>46.366999999999997</v>
+      </c>
+      <c r="E17" s="9">
+        <v>17.885000000000002</v>
+      </c>
+      <c r="F17" s="9">
+        <f t="shared" si="0"/>
+        <v>13.573999999999998</v>
+      </c>
+      <c r="G17" s="9">
+        <f t="shared" si="1"/>
+        <v>9.6020000000000021</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="9">
+        <v>2078.692</v>
+      </c>
+      <c r="C18" s="9">
+        <v>5043.7969999999996</v>
+      </c>
+      <c r="D18" s="9">
+        <v>34612.029000000002</v>
+      </c>
+      <c r="E18" s="9">
+        <v>80644.687999999995</v>
+      </c>
+      <c r="F18" s="9">
+        <f t="shared" si="0"/>
+        <v>32533.337000000003</v>
+      </c>
+      <c r="G18" s="9">
+        <f t="shared" si="1"/>
+        <v>75600.890999999989</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="9">
+        <v>37.951999999999998</v>
+      </c>
+      <c r="C19" s="9">
+        <v>16.440999999999999</v>
+      </c>
+      <c r="D19" s="9">
+        <v>52.209000000000003</v>
+      </c>
+      <c r="E19" s="9">
+        <v>19.71</v>
+      </c>
+      <c r="F19" s="9">
+        <f t="shared" si="0"/>
+        <v>14.257000000000005</v>
+      </c>
+      <c r="G19" s="9">
+        <f t="shared" si="1"/>
+        <v>3.2690000000000019</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="9">
+        <v>2704.201</v>
+      </c>
+      <c r="C20" s="9">
+        <v>5105.7370000000001</v>
+      </c>
+      <c r="D20" s="9">
+        <v>7555.1139999999996</v>
+      </c>
+      <c r="E20" s="9">
+        <v>9615.5329999999994</v>
+      </c>
+      <c r="F20" s="9">
+        <f t="shared" si="0"/>
+        <v>4850.9129999999996</v>
+      </c>
+      <c r="G20" s="9">
+        <f t="shared" si="1"/>
+        <v>4509.7959999999994</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="9">
+        <v>10724.819</v>
+      </c>
+      <c r="C21" s="9">
+        <v>23780.648000000001</v>
+      </c>
+      <c r="D21" s="9">
+        <v>11330.832</v>
+      </c>
+      <c r="E21" s="9">
+        <v>21074.595000000001</v>
+      </c>
+      <c r="F21" s="9">
+        <f t="shared" si="0"/>
+        <v>606.01300000000083</v>
+      </c>
+      <c r="G21" s="9">
+        <f t="shared" si="1"/>
+        <v>-2706.0529999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="9">
+        <v>465.48200000000003</v>
+      </c>
+      <c r="C22" s="9">
+        <v>48.981999999999999</v>
+      </c>
+      <c r="D22" s="9">
+        <v>60.277999999999999</v>
+      </c>
+      <c r="E22" s="9">
+        <v>22.177</v>
+      </c>
+      <c r="F22" s="9">
+        <f t="shared" si="0"/>
+        <v>-405.20400000000001</v>
+      </c>
+      <c r="G22" s="9">
+        <f t="shared" si="1"/>
+        <v>-26.805</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="9">
+        <v>20345.02</v>
+      </c>
+      <c r="C23" s="9">
+        <v>4222.9229999999998</v>
+      </c>
+      <c r="D23" s="9">
+        <v>43.067999999999998</v>
+      </c>
+      <c r="E23" s="9">
+        <v>25.419</v>
+      </c>
+      <c r="F23" s="9">
+        <f t="shared" si="0"/>
+        <v>-20301.952000000001</v>
+      </c>
+      <c r="G23" s="9">
+        <f t="shared" si="1"/>
+        <v>-4197.5039999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="9">
+        <v>26.148</v>
+      </c>
+      <c r="C24" s="9">
+        <v>24.606999999999999</v>
+      </c>
+      <c r="D24" s="9">
+        <v>20.09</v>
+      </c>
+      <c r="E24" s="9">
+        <v>15.574</v>
+      </c>
+      <c r="F24" s="9">
+        <f t="shared" si="0"/>
+        <v>-6.0579999999999998</v>
+      </c>
+      <c r="G24" s="9">
+        <f t="shared" si="1"/>
+        <v>-9.0329999999999995</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" s="9">
+        <v>6.8739999999999997</v>
+      </c>
+      <c r="C25" s="9">
+        <v>1.5509999999999999</v>
+      </c>
+      <c r="D25" s="9">
+        <v>7.1509999999999998</v>
+      </c>
+      <c r="E25" s="9">
+        <v>1.292</v>
+      </c>
+      <c r="F25" s="9">
+        <f t="shared" si="0"/>
+        <v>0.27700000000000014</v>
+      </c>
+      <c r="G25" s="9">
+        <f t="shared" si="1"/>
+        <v>-0.2589999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="F3:G25">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="30.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="10.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="7"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="6"/>
+      <c r="B2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>10.631</v>
+      </c>
+      <c r="C3">
+        <v>3.117</v>
+      </c>
+      <c r="D3">
+        <v>15.577999999999999</v>
+      </c>
+      <c r="E3">
+        <v>7.5519999999999996</v>
+      </c>
+      <c r="F3">
+        <f>D3-B3</f>
+        <v>4.9469999999999992</v>
+      </c>
+      <c r="G3">
+        <f>E3-C3</f>
+        <v>4.4349999999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>4.8769999999999998</v>
+      </c>
+      <c r="C4">
+        <v>2.8159999999999998</v>
+      </c>
+      <c r="D4">
+        <v>6.2750000000000004</v>
+      </c>
+      <c r="E4">
+        <v>2.5939999999999999</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ref="F4:F25" si="0">D4-B4</f>
+        <v>1.3980000000000006</v>
+      </c>
+      <c r="G4">
+        <f t="shared" ref="G4:G25" si="1">E4-C4</f>
+        <v>-0.22199999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>15.311999999999999</v>
+      </c>
+      <c r="C5">
+        <v>2.4449999999999998</v>
+      </c>
+      <c r="D5">
+        <v>15.603</v>
+      </c>
+      <c r="E5">
+        <v>2.617</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>0.29100000000000037</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>0.17200000000000015</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>16.405999999999999</v>
+      </c>
+      <c r="C6">
+        <v>1.66</v>
+      </c>
+      <c r="D6">
+        <v>16.638999999999999</v>
+      </c>
+      <c r="E6">
+        <v>1.794</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>0.23300000000000054</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>0.13400000000000012</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>22.771999999999998</v>
+      </c>
+      <c r="C7">
+        <v>1.9</v>
+      </c>
+      <c r="D7">
+        <v>23.074000000000002</v>
+      </c>
+      <c r="E7">
+        <v>2.452</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>0.30200000000000315</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>0.55200000000000005</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>80.492999999999995</v>
+      </c>
+      <c r="C8">
+        <v>70.14</v>
+      </c>
+      <c r="D8">
+        <v>140.398</v>
+      </c>
+      <c r="E8">
+        <v>164.512</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>59.905000000000001</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>94.372</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>175.11799999999999</v>
+      </c>
+      <c r="C9">
+        <v>86.63</v>
+      </c>
+      <c r="D9">
+        <v>175.19200000000001</v>
+      </c>
+      <c r="E9">
+        <v>102.43600000000001</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>7.4000000000012278E-2</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>15.806000000000012</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>421.72199999999998</v>
+      </c>
+      <c r="C10">
+        <v>566.70600000000002</v>
+      </c>
+      <c r="D10">
+        <v>974.70299999999997</v>
+      </c>
+      <c r="E10">
+        <v>1767.164</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>552.98099999999999</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>1200.4580000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>73.715999999999994</v>
+      </c>
+      <c r="C11">
+        <v>22.920999999999999</v>
+      </c>
+      <c r="D11">
+        <v>105.697</v>
+      </c>
+      <c r="E11">
+        <v>123.83</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>31.981000000000009</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>100.90899999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>666.88499999999999</v>
+      </c>
+      <c r="C12">
+        <v>597.20500000000004</v>
+      </c>
+      <c r="D12">
+        <v>773.72799999999995</v>
+      </c>
+      <c r="E12">
+        <v>649.99599999999998</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>106.84299999999996</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>52.79099999999994</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>12.346</v>
+      </c>
+      <c r="C13">
+        <v>2.016</v>
+      </c>
+      <c r="D13">
+        <v>12.085000000000001</v>
+      </c>
+      <c r="E13">
+        <v>1.825</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>-0.26099999999999923</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>-0.19100000000000006</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14">
+        <v>5.3819999999999997</v>
+      </c>
+      <c r="C14">
+        <v>0.46899999999999997</v>
+      </c>
+      <c r="D14">
+        <v>5.5060000000000002</v>
+      </c>
+      <c r="E14">
+        <v>0.38600000000000001</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>0.12400000000000055</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>-8.2999999999999963E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15">
+        <v>43.822000000000003</v>
+      </c>
+      <c r="C15">
+        <v>20.204000000000001</v>
+      </c>
+      <c r="D15">
+        <v>42.78</v>
+      </c>
+      <c r="E15">
+        <v>25.027999999999999</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>-1.0420000000000016</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="1"/>
+        <v>4.8239999999999981</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16">
+        <v>2736.5039999999999</v>
+      </c>
+      <c r="C16">
+        <v>9593.1029999999992</v>
+      </c>
+      <c r="D16">
+        <v>9971.4670000000006</v>
+      </c>
+      <c r="E16">
+        <v>22948.815999999999</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>7234.9630000000006</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="1"/>
+        <v>13355.713</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17">
+        <v>47.225999999999999</v>
+      </c>
+      <c r="C17">
+        <v>21.035</v>
+      </c>
+      <c r="D17">
+        <v>32.783999999999999</v>
+      </c>
+      <c r="E17">
+        <v>16.023</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>-14.442</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="1"/>
+        <v>-5.0120000000000005</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18">
+        <v>8762.3119999999999</v>
+      </c>
+      <c r="C18">
+        <v>21273.763999999999</v>
+      </c>
+      <c r="D18">
+        <v>18080.294999999998</v>
+      </c>
+      <c r="E18">
+        <v>33439.836000000003</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>9317.9829999999984</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="1"/>
+        <v>12166.072000000004</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19">
+        <v>38.439</v>
+      </c>
+      <c r="C19">
+        <v>16.495999999999999</v>
+      </c>
+      <c r="D19">
+        <v>40.970999999999997</v>
+      </c>
+      <c r="E19">
+        <v>21.065000000000001</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>2.5319999999999965</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="1"/>
+        <v>4.5690000000000026</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20">
+        <v>2525.9340000000002</v>
+      </c>
+      <c r="C20">
+        <v>6143.7520000000004</v>
+      </c>
+      <c r="D20">
+        <v>10131.306</v>
+      </c>
+      <c r="E20">
+        <v>32293.994999999999</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>7605.3720000000003</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="1"/>
+        <v>26150.242999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21">
+        <v>8886.152</v>
+      </c>
+      <c r="C21">
+        <v>21363.901000000002</v>
+      </c>
+      <c r="D21">
+        <v>15462.945</v>
+      </c>
+      <c r="E21">
+        <v>40948.423999999999</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>6576.7929999999997</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="1"/>
+        <v>19584.522999999997</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22">
+        <v>62.408999999999999</v>
+      </c>
+      <c r="C22">
+        <v>22.071999999999999</v>
+      </c>
+      <c r="D22">
+        <v>67.814999999999998</v>
+      </c>
+      <c r="E22">
+        <v>28.277000000000001</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>5.4059999999999988</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="1"/>
+        <v>6.2050000000000018</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23">
+        <v>35.935000000000002</v>
+      </c>
+      <c r="C23">
+        <v>29.437999999999999</v>
+      </c>
+      <c r="D23">
+        <v>37.154000000000003</v>
+      </c>
+      <c r="E23">
+        <v>25.332000000000001</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>1.2190000000000012</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="1"/>
+        <v>-4.1059999999999981</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24">
+        <v>23.021999999999998</v>
+      </c>
+      <c r="C24">
+        <v>20.852</v>
+      </c>
+      <c r="D24">
+        <v>21.375</v>
+      </c>
+      <c r="E24">
+        <v>21.225000000000001</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="0"/>
+        <v>-1.6469999999999985</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="1"/>
+        <v>0.37300000000000111</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25">
+        <v>6.5570000000000004</v>
+      </c>
+      <c r="C25">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="D25">
+        <v>6.6109999999999998</v>
+      </c>
+      <c r="E25">
+        <v>1.375</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="0"/>
+        <v>5.3999999999999382E-2</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="1"/>
+        <v>0.21500000000000008</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="F3:G25">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:G23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="32.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>10.496</v>
+      </c>
+      <c r="C3">
+        <v>2.839</v>
+      </c>
+      <c r="D3">
+        <v>13.875999999999999</v>
+      </c>
+      <c r="E3">
+        <v>5.2039999999999997</v>
+      </c>
+      <c r="F3">
+        <f>D3-B3</f>
+        <v>3.379999999999999</v>
+      </c>
+      <c r="G3">
+        <f>E3-C3</f>
+        <v>2.3649999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>5.0119999999999996</v>
+      </c>
+      <c r="C4">
+        <v>3.3620000000000001</v>
+      </c>
+      <c r="D4">
+        <v>6.4790000000000001</v>
+      </c>
+      <c r="E4">
+        <v>3.589</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ref="F4:F23" si="0">D4-B4</f>
+        <v>1.4670000000000005</v>
+      </c>
+      <c r="G4">
+        <f t="shared" ref="G4:G23" si="1">E4-C4</f>
+        <v>0.22699999999999987</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>16.311</v>
+      </c>
+      <c r="C5">
+        <v>4.1369999999999996</v>
+      </c>
+      <c r="D5">
+        <v>16.071999999999999</v>
+      </c>
+      <c r="E5">
+        <v>4.6440000000000001</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>-0.23900000000000077</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>0.50700000000000056</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>16.082999999999998</v>
+      </c>
+      <c r="C6">
+        <v>1.65</v>
+      </c>
+      <c r="D6">
+        <v>16.279</v>
+      </c>
+      <c r="E6">
+        <v>1.8420000000000001</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>0.19600000000000151</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>0.19200000000000017</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>22.314</v>
+      </c>
+      <c r="C7">
+        <v>2.782</v>
+      </c>
+      <c r="D7">
+        <v>23.446999999999999</v>
+      </c>
+      <c r="E7">
+        <v>3.1749999999999998</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>1.1329999999999991</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>0.39299999999999979</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>99.323999999999998</v>
+      </c>
+      <c r="C8">
+        <v>114.074</v>
+      </c>
+      <c r="D8">
+        <v>87.216999999999999</v>
+      </c>
+      <c r="E8">
+        <v>86.685000000000002</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>-12.106999999999999</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>-27.388999999999996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>156.03399999999999</v>
+      </c>
+      <c r="C9">
+        <v>91.278999999999996</v>
+      </c>
+      <c r="D9">
+        <v>174.86199999999999</v>
+      </c>
+      <c r="E9">
+        <v>120.748</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>18.828000000000003</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>29.469000000000008</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>544.11199999999997</v>
+      </c>
+      <c r="C10">
+        <v>786.01499999999999</v>
+      </c>
+      <c r="D10">
+        <v>1235.354</v>
+      </c>
+      <c r="E10">
+        <v>2613.777</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>691.24200000000008</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>1827.7620000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>76.129000000000005</v>
+      </c>
+      <c r="C11">
+        <v>29.524999999999999</v>
+      </c>
+      <c r="D11">
+        <v>94.105000000000004</v>
+      </c>
+      <c r="E11">
+        <v>65.692999999999998</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>17.975999999999999</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>36.167999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>741.50400000000002</v>
+      </c>
+      <c r="C12">
+        <v>1273.5999999999999</v>
+      </c>
+      <c r="D12">
+        <v>733.41200000000003</v>
+      </c>
+      <c r="E12">
+        <v>581.077</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>-8.0919999999999845</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>-692.52299999999991</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>22.791</v>
+      </c>
+      <c r="C13">
+        <v>1.847</v>
+      </c>
+      <c r="D13">
+        <v>12.757</v>
+      </c>
+      <c r="E13">
+        <v>2.09</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>-10.034000000000001</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>0.24299999999999988</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14">
+        <v>5.4749999999999996</v>
+      </c>
+      <c r="C14">
+        <v>0.373</v>
+      </c>
+      <c r="D14">
+        <v>5.556</v>
+      </c>
+      <c r="E14">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>8.1000000000000405E-2</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>1.2000000000000011E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15">
+        <v>37.442999999999998</v>
+      </c>
+      <c r="C15">
+        <v>20.876999999999999</v>
+      </c>
+      <c r="D15">
+        <v>47.468000000000004</v>
+      </c>
+      <c r="E15">
+        <v>20.724</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>10.025000000000006</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="1"/>
+        <v>-0.15299999999999869</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16">
+        <v>9174.9609999999993</v>
+      </c>
+      <c r="C16">
+        <v>20534.129000000001</v>
+      </c>
+      <c r="D16">
+        <v>7345.5969999999998</v>
+      </c>
+      <c r="E16">
+        <v>29469.362000000001</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>-1829.3639999999996</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="1"/>
+        <v>8935.2330000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17">
+        <v>41.118000000000002</v>
+      </c>
+      <c r="C17">
+        <v>21.097000000000001</v>
+      </c>
+      <c r="D17">
+        <v>37.796999999999997</v>
+      </c>
+      <c r="E17">
+        <v>19.867999999999999</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>-3.3210000000000051</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="1"/>
+        <v>-1.2290000000000028</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18">
+        <v>12544.933999999999</v>
+      </c>
+      <c r="C18">
+        <v>29430.321</v>
+      </c>
+      <c r="D18">
+        <v>13782.712</v>
+      </c>
+      <c r="E18">
+        <v>38496.542999999998</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>1237.7780000000002</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="1"/>
+        <v>9066.2219999999979</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19">
+        <v>43.286999999999999</v>
+      </c>
+      <c r="C19">
+        <v>23.895</v>
+      </c>
+      <c r="D19">
+        <v>39.136000000000003</v>
+      </c>
+      <c r="E19">
+        <v>19.056000000000001</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>-4.1509999999999962</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="1"/>
+        <v>-4.8389999999999986</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20">
+        <v>2444.9540000000002</v>
+      </c>
+      <c r="C20">
+        <v>5708.1549999999997</v>
+      </c>
+      <c r="D20">
+        <v>4584.5510000000004</v>
+      </c>
+      <c r="E20">
+        <v>11710.708000000001</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>2139.5970000000002</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="1"/>
+        <v>6002.5530000000008</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21">
+        <v>3635.1529999999998</v>
+      </c>
+      <c r="C21">
+        <v>7537.7569999999996</v>
+      </c>
+      <c r="D21">
+        <v>1461.028</v>
+      </c>
+      <c r="E21">
+        <v>3492.107</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>-2174.125</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="1"/>
+        <v>-4045.6499999999996</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22">
+        <v>474.78199999999998</v>
+      </c>
+      <c r="C22">
+        <v>43.686</v>
+      </c>
+      <c r="D22">
+        <v>63.359000000000002</v>
+      </c>
+      <c r="E22">
+        <v>24.827000000000002</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>-411.423</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="1"/>
+        <v>-18.858999999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23">
+        <v>23990.053</v>
+      </c>
+      <c r="C23">
+        <v>5655.3729999999996</v>
+      </c>
+      <c r="D23">
+        <v>37.609000000000002</v>
+      </c>
+      <c r="E23">
+        <v>20.792000000000002</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>-23952.444</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="1"/>
+        <v>-5634.5809999999992</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="F3:G23">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>